<commit_message>
Added Scripts in Reports module and updated the framework
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,18 +4,30 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20623" windowHeight="4420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +343,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>